<commit_message>
add new filter rule
</commit_message>
<xml_diff>
--- a/config/excelConfig.xlsx
+++ b/config/excelConfig.xlsx
@@ -215,23 +215,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>磷酸铁锂</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\330change.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\330output.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>镍钴锰</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>磷酸铁锂</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D:\330change.xlsx</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D:\330output.xlsx</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -819,7 +819,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>48</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>46</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>39</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>47</v>

</xml_diff>